<commit_message>
ajout categorie SINP et update formaulires
</commit_message>
<xml_diff>
--- a/docs/ODK-CEN/fichiers/SicenODK/Sicen_2022.xlsx
+++ b/docs/ODK-CEN/fichiers/SicenODK/Sicen_2022.xlsx
@@ -2618,13 +2618,13 @@
   </sheetPr>
   <dimension ref="A1:S219"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="2:220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.65234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="4.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.71"/>
@@ -5341,12 +5341,12 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A228" activeCellId="0" sqref="A228"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="2:220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.56"/>
@@ -7980,10 +7980,10 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:220"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
@@ -8052,10 +8052,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A41" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8714,6 +8714,7 @@
         <v>806</v>
       </c>
     </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>